<commit_message>
Updated models.  Added new categories and companies
</commit_message>
<xml_diff>
--- a/BASE_MODEL.xlsx
+++ b/BASE_MODEL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2560B828-A891-4F56-AE0A-5CBEFC277928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64D842D-1FBB-403F-85DA-F6CE58FB2993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{74C982A1-EE30-4588-AA95-0E58E4E415F0}"/>
   </bookViews>
@@ -65,40 +65,6 @@
           </rPr>
           <t xml:space="preserve">
 Long Term Debt</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Alex</author>
-  </authors>
-  <commentList>
-    <comment ref="X12" authorId="0" shapeId="0" xr:uid="{8EF501D2-921F-4122-992C-604E40734CA8}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Alex:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Supply chain optimization costs</t>
         </r>
       </text>
     </comment>
@@ -484,7 +450,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -528,11 +494,10 @@
     <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -872,7 +837,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -918,6 +883,10 @@
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B6" s="1">
+        <f>B4*B5</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -935,6 +904,10 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <f>B6-B7+B8</f>
+        <v>0</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>27</v>
@@ -947,11 +920,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E38C8F-3B6A-4584-925C-61BD108C4B76}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E38C8F-3B6A-4584-925C-61BD108C4B76}">
   <dimension ref="A1:AH77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N43" sqref="N43"/>
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -1155,7 +1128,7 @@
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4">
-        <f t="shared" ref="D10:G10" si="0">D8 -D9</f>
+        <f t="shared" ref="D10:F10" si="0">D8 -D9</f>
         <v>0</v>
       </c>
       <c r="E10" s="4">
@@ -1167,10 +1140,11 @@
         <v>0</v>
       </c>
       <c r="G10" s="4">
-        <v>440</v>
+        <f t="shared" ref="G10:K10" si="1">G8 -G9</f>
+        <v>0</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" ref="H10:K10" si="1">H8 -H9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I10" s="4">
@@ -1334,7 +1308,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="4">
-        <f t="shared" ref="D14:G14" si="3">D10-SUM(D11:D13)</f>
+        <f t="shared" ref="D14:F14" si="3">D10-SUM(D11:D13)</f>
         <v>0</v>
       </c>
       <c r="E14" s="4">
@@ -1346,8 +1320,8 @@
         <v>0</v>
       </c>
       <c r="G14" s="4">
-        <f t="shared" si="3"/>
-        <v>440</v>
+        <f>G10-SUM(G11:G13)</f>
+        <v>0</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" ref="H14:K14" si="4">H10-SUM(H11:H13)</f>
@@ -1576,91 +1550,91 @@
       <c r="U19" s="29"/>
       <c r="V19" s="29"/>
     </row>
-    <row r="21" spans="2:25" s="36" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="36" t="s">
+    <row r="21" spans="2:25" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="36" t="s">
+      <c r="E21" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="F21" s="36" t="s">
+      <c r="F21" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="G21" s="36" t="s">
+      <c r="G21" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="H21" s="37" t="e">
+      <c r="H21" s="34" t="e">
         <f t="shared" ref="H21" si="11">(H8/D8) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I21" s="37" t="e">
+      <c r="I21" s="34" t="e">
         <f t="shared" ref="I21" si="12">(I8/E8) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J21" s="37" t="e">
+      <c r="J21" s="34" t="e">
         <f t="shared" ref="J21" si="13">(J8/F8) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K21" s="37" t="e">
+      <c r="K21" s="34" t="e">
         <f t="shared" ref="K21" si="14">(K8/G8) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L21" s="37" t="e">
+      <c r="L21" s="34" t="e">
         <f t="shared" ref="L21" si="15">(L8/H8) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M21" s="37" t="e">
+      <c r="M21" s="34" t="e">
         <f t="shared" ref="M21" si="16">(M8/I8) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N21" s="37" t="e">
+      <c r="N21" s="34" t="e">
         <f t="shared" ref="N21" si="17">(N8/J8) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O21" s="37" t="e">
+      <c r="O21" s="34" t="e">
         <f t="shared" ref="O21" si="18">(O8/K8) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P21" s="37" t="e">
+      <c r="P21" s="34" t="e">
         <f t="shared" ref="P21" si="19">(P8/L8) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q21" s="37" t="e">
+      <c r="Q21" s="34" t="e">
         <f t="shared" ref="Q21" si="20">(Q8/M8) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R21" s="37" t="e">
+      <c r="R21" s="34" t="e">
         <f t="shared" ref="R21:Y21" si="21">(R8/N8) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S21" s="37" t="e">
+      <c r="S21" s="34" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="T21" s="37" t="e">
+      <c r="T21" s="34" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="U21" s="37" t="e">
+      <c r="U21" s="34" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="V21" s="37" t="e">
+      <c r="V21" s="34" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="W21" s="37" t="e">
+      <c r="W21" s="34" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="X21" s="37" t="e">
+      <c r="X21" s="34" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y21" s="37" t="e">
+      <c r="Y21" s="34" t="e">
         <f t="shared" si="21"/>
         <v>#DIV/0!</v>
       </c>
@@ -2206,14 +2180,6 @@
     <row r="46" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B46" s="11"/>
       <c r="C46" s="12"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="35"/>
-      <c r="I46" s="35"/>
-      <c r="J46" s="35"/>
-      <c r="K46" s="35"/>
     </row>
     <row r="47" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B47" s="15"/>
@@ -2227,14 +2193,6 @@
     <row r="50" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B50" s="18"/>
       <c r="C50" s="19"/>
-      <c r="D50" s="35"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="35"/>
-      <c r="H50" s="35"/>
-      <c r="I50" s="35"/>
-      <c r="J50" s="35"/>
-      <c r="K50" s="35"/>
     </row>
     <row r="51" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="2:34" x14ac:dyDescent="0.2">
@@ -2278,353 +2236,353 @@
     </row>
     <row r="54" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="15"/>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="33"/>
-      <c r="H54" s="33"/>
-      <c r="I54" s="33"/>
-      <c r="J54" s="33"/>
-      <c r="K54" s="33"/>
-      <c r="L54" s="33"/>
-      <c r="M54" s="33"/>
-      <c r="N54" s="33"/>
-      <c r="O54" s="33"/>
-      <c r="P54" s="33"/>
-      <c r="Q54" s="33"/>
-      <c r="R54" s="33"/>
-      <c r="S54" s="33"/>
-      <c r="T54" s="33"/>
-      <c r="U54" s="33"/>
-      <c r="V54" s="33"/>
-      <c r="W54" s="33"/>
-      <c r="X54" s="33"/>
-      <c r="Y54" s="33"/>
-      <c r="Z54" s="33"/>
-      <c r="AA54" s="33"/>
-      <c r="AB54" s="33"/>
-      <c r="AC54" s="33"/>
-      <c r="AD54" s="33"/>
-      <c r="AE54" s="33"/>
-      <c r="AF54" s="33"/>
-      <c r="AG54" s="33"/>
-      <c r="AH54" s="34"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="35"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="35"/>
+      <c r="K54" s="35"/>
+      <c r="L54" s="35"/>
+      <c r="M54" s="35"/>
+      <c r="N54" s="35"/>
+      <c r="O54" s="35"/>
+      <c r="P54" s="35"/>
+      <c r="Q54" s="35"/>
+      <c r="R54" s="35"/>
+      <c r="S54" s="35"/>
+      <c r="T54" s="35"/>
+      <c r="U54" s="35"/>
+      <c r="V54" s="35"/>
+      <c r="W54" s="35"/>
+      <c r="X54" s="35"/>
+      <c r="Y54" s="35"/>
+      <c r="Z54" s="35"/>
+      <c r="AA54" s="35"/>
+      <c r="AB54" s="35"/>
+      <c r="AC54" s="35"/>
+      <c r="AD54" s="35"/>
+      <c r="AE54" s="35"/>
+      <c r="AF54" s="35"/>
+      <c r="AG54" s="35"/>
+      <c r="AH54" s="36"/>
     </row>
     <row r="55" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="15"/>
-      <c r="C55" s="33"/>
-      <c r="D55" s="33"/>
-      <c r="E55" s="33"/>
-      <c r="F55" s="33"/>
-      <c r="G55" s="33"/>
-      <c r="H55" s="33"/>
-      <c r="I55" s="33"/>
-      <c r="J55" s="33"/>
-      <c r="K55" s="33"/>
-      <c r="L55" s="33"/>
-      <c r="M55" s="33"/>
-      <c r="N55" s="33"/>
-      <c r="O55" s="33"/>
-      <c r="P55" s="33"/>
-      <c r="Q55" s="33"/>
-      <c r="R55" s="33"/>
-      <c r="S55" s="33"/>
-      <c r="T55" s="33"/>
-      <c r="U55" s="33"/>
-      <c r="V55" s="33"/>
-      <c r="W55" s="33"/>
-      <c r="X55" s="33"/>
-      <c r="Y55" s="33"/>
-      <c r="Z55" s="33"/>
-      <c r="AA55" s="33"/>
-      <c r="AB55" s="33"/>
-      <c r="AC55" s="33"/>
-      <c r="AD55" s="33"/>
-      <c r="AE55" s="33"/>
-      <c r="AF55" s="33"/>
-      <c r="AG55" s="33"/>
-      <c r="AH55" s="34"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="35"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="35"/>
+      <c r="K55" s="35"/>
+      <c r="L55" s="35"/>
+      <c r="M55" s="35"/>
+      <c r="N55" s="35"/>
+      <c r="O55" s="35"/>
+      <c r="P55" s="35"/>
+      <c r="Q55" s="35"/>
+      <c r="R55" s="35"/>
+      <c r="S55" s="35"/>
+      <c r="T55" s="35"/>
+      <c r="U55" s="35"/>
+      <c r="V55" s="35"/>
+      <c r="W55" s="35"/>
+      <c r="X55" s="35"/>
+      <c r="Y55" s="35"/>
+      <c r="Z55" s="35"/>
+      <c r="AA55" s="35"/>
+      <c r="AB55" s="35"/>
+      <c r="AC55" s="35"/>
+      <c r="AD55" s="35"/>
+      <c r="AE55" s="35"/>
+      <c r="AF55" s="35"/>
+      <c r="AG55" s="35"/>
+      <c r="AH55" s="36"/>
     </row>
     <row r="56" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="15"/>
-      <c r="C56" s="33"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="33"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="33"/>
-      <c r="H56" s="33"/>
-      <c r="I56" s="33"/>
-      <c r="J56" s="33"/>
-      <c r="K56" s="33"/>
-      <c r="L56" s="33"/>
-      <c r="M56" s="33"/>
-      <c r="N56" s="33"/>
-      <c r="O56" s="33"/>
-      <c r="P56" s="33"/>
-      <c r="Q56" s="33"/>
-      <c r="R56" s="33"/>
-      <c r="S56" s="33"/>
-      <c r="T56" s="33"/>
-      <c r="U56" s="33"/>
-      <c r="V56" s="33"/>
-      <c r="W56" s="33"/>
-      <c r="X56" s="33"/>
-      <c r="Y56" s="33"/>
-      <c r="Z56" s="33"/>
-      <c r="AA56" s="33"/>
-      <c r="AB56" s="33"/>
-      <c r="AC56" s="33"/>
-      <c r="AD56" s="33"/>
-      <c r="AE56" s="33"/>
-      <c r="AF56" s="33"/>
-      <c r="AG56" s="33"/>
-      <c r="AH56" s="34"/>
+      <c r="C56" s="35"/>
+      <c r="D56" s="35"/>
+      <c r="E56" s="35"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="35"/>
+      <c r="H56" s="35"/>
+      <c r="I56" s="35"/>
+      <c r="J56" s="35"/>
+      <c r="K56" s="35"/>
+      <c r="L56" s="35"/>
+      <c r="M56" s="35"/>
+      <c r="N56" s="35"/>
+      <c r="O56" s="35"/>
+      <c r="P56" s="35"/>
+      <c r="Q56" s="35"/>
+      <c r="R56" s="35"/>
+      <c r="S56" s="35"/>
+      <c r="T56" s="35"/>
+      <c r="U56" s="35"/>
+      <c r="V56" s="35"/>
+      <c r="W56" s="35"/>
+      <c r="X56" s="35"/>
+      <c r="Y56" s="35"/>
+      <c r="Z56" s="35"/>
+      <c r="AA56" s="35"/>
+      <c r="AB56" s="35"/>
+      <c r="AC56" s="35"/>
+      <c r="AD56" s="35"/>
+      <c r="AE56" s="35"/>
+      <c r="AF56" s="35"/>
+      <c r="AG56" s="35"/>
+      <c r="AH56" s="36"/>
     </row>
     <row r="57" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="15"/>
-      <c r="C57" s="33"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="33"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="33"/>
-      <c r="H57" s="33"/>
-      <c r="I57" s="33"/>
-      <c r="J57" s="33"/>
-      <c r="K57" s="33"/>
-      <c r="L57" s="33"/>
-      <c r="M57" s="33"/>
-      <c r="N57" s="33"/>
-      <c r="O57" s="33"/>
-      <c r="P57" s="33"/>
-      <c r="Q57" s="33"/>
-      <c r="R57" s="33"/>
-      <c r="S57" s="33"/>
-      <c r="T57" s="33"/>
-      <c r="U57" s="33"/>
-      <c r="V57" s="33"/>
-      <c r="W57" s="33"/>
-      <c r="X57" s="33"/>
-      <c r="Y57" s="33"/>
-      <c r="Z57" s="33"/>
-      <c r="AA57" s="33"/>
-      <c r="AB57" s="33"/>
-      <c r="AC57" s="33"/>
-      <c r="AD57" s="33"/>
-      <c r="AE57" s="33"/>
-      <c r="AF57" s="33"/>
-      <c r="AG57" s="33"/>
-      <c r="AH57" s="34"/>
+      <c r="C57" s="35"/>
+      <c r="D57" s="35"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="35"/>
+      <c r="H57" s="35"/>
+      <c r="I57" s="35"/>
+      <c r="J57" s="35"/>
+      <c r="K57" s="35"/>
+      <c r="L57" s="35"/>
+      <c r="M57" s="35"/>
+      <c r="N57" s="35"/>
+      <c r="O57" s="35"/>
+      <c r="P57" s="35"/>
+      <c r="Q57" s="35"/>
+      <c r="R57" s="35"/>
+      <c r="S57" s="35"/>
+      <c r="T57" s="35"/>
+      <c r="U57" s="35"/>
+      <c r="V57" s="35"/>
+      <c r="W57" s="35"/>
+      <c r="X57" s="35"/>
+      <c r="Y57" s="35"/>
+      <c r="Z57" s="35"/>
+      <c r="AA57" s="35"/>
+      <c r="AB57" s="35"/>
+      <c r="AC57" s="35"/>
+      <c r="AD57" s="35"/>
+      <c r="AE57" s="35"/>
+      <c r="AF57" s="35"/>
+      <c r="AG57" s="35"/>
+      <c r="AH57" s="36"/>
     </row>
     <row r="58" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="15"/>
-      <c r="C58" s="33"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="33"/>
-      <c r="G58" s="33"/>
-      <c r="H58" s="33"/>
-      <c r="I58" s="33"/>
-      <c r="J58" s="33"/>
-      <c r="K58" s="33"/>
-      <c r="L58" s="33"/>
-      <c r="M58" s="33"/>
-      <c r="N58" s="33"/>
-      <c r="O58" s="33"/>
-      <c r="P58" s="33"/>
-      <c r="Q58" s="33"/>
-      <c r="R58" s="33"/>
-      <c r="S58" s="33"/>
-      <c r="T58" s="33"/>
-      <c r="U58" s="33"/>
-      <c r="V58" s="33"/>
-      <c r="W58" s="33"/>
-      <c r="X58" s="33"/>
-      <c r="Y58" s="33"/>
-      <c r="Z58" s="33"/>
-      <c r="AA58" s="33"/>
-      <c r="AB58" s="33"/>
-      <c r="AC58" s="33"/>
-      <c r="AD58" s="33"/>
-      <c r="AE58" s="33"/>
-      <c r="AF58" s="33"/>
-      <c r="AG58" s="33"/>
-      <c r="AH58" s="34"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="35"/>
+      <c r="H58" s="35"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="35"/>
+      <c r="K58" s="35"/>
+      <c r="L58" s="35"/>
+      <c r="M58" s="35"/>
+      <c r="N58" s="35"/>
+      <c r="O58" s="35"/>
+      <c r="P58" s="35"/>
+      <c r="Q58" s="35"/>
+      <c r="R58" s="35"/>
+      <c r="S58" s="35"/>
+      <c r="T58" s="35"/>
+      <c r="U58" s="35"/>
+      <c r="V58" s="35"/>
+      <c r="W58" s="35"/>
+      <c r="X58" s="35"/>
+      <c r="Y58" s="35"/>
+      <c r="Z58" s="35"/>
+      <c r="AA58" s="35"/>
+      <c r="AB58" s="35"/>
+      <c r="AC58" s="35"/>
+      <c r="AD58" s="35"/>
+      <c r="AE58" s="35"/>
+      <c r="AF58" s="35"/>
+      <c r="AG58" s="35"/>
+      <c r="AH58" s="36"/>
     </row>
     <row r="59" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B59" s="15"/>
-      <c r="C59" s="33"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="33"/>
-      <c r="H59" s="33"/>
-      <c r="I59" s="33"/>
-      <c r="J59" s="33"/>
-      <c r="K59" s="33"/>
-      <c r="L59" s="33"/>
-      <c r="M59" s="33"/>
-      <c r="N59" s="33"/>
-      <c r="O59" s="33"/>
-      <c r="P59" s="33"/>
-      <c r="Q59" s="33"/>
-      <c r="R59" s="33"/>
-      <c r="S59" s="33"/>
-      <c r="T59" s="33"/>
-      <c r="U59" s="33"/>
-      <c r="V59" s="33"/>
-      <c r="W59" s="33"/>
-      <c r="X59" s="33"/>
-      <c r="Y59" s="33"/>
-      <c r="Z59" s="33"/>
-      <c r="AA59" s="33"/>
-      <c r="AB59" s="33"/>
-      <c r="AC59" s="33"/>
-      <c r="AD59" s="33"/>
-      <c r="AE59" s="33"/>
-      <c r="AF59" s="33"/>
-      <c r="AG59" s="33"/>
-      <c r="AH59" s="34"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="35"/>
+      <c r="G59" s="35"/>
+      <c r="H59" s="35"/>
+      <c r="I59" s="35"/>
+      <c r="J59" s="35"/>
+      <c r="K59" s="35"/>
+      <c r="L59" s="35"/>
+      <c r="M59" s="35"/>
+      <c r="N59" s="35"/>
+      <c r="O59" s="35"/>
+      <c r="P59" s="35"/>
+      <c r="Q59" s="35"/>
+      <c r="R59" s="35"/>
+      <c r="S59" s="35"/>
+      <c r="T59" s="35"/>
+      <c r="U59" s="35"/>
+      <c r="V59" s="35"/>
+      <c r="W59" s="35"/>
+      <c r="X59" s="35"/>
+      <c r="Y59" s="35"/>
+      <c r="Z59" s="35"/>
+      <c r="AA59" s="35"/>
+      <c r="AB59" s="35"/>
+      <c r="AC59" s="35"/>
+      <c r="AD59" s="35"/>
+      <c r="AE59" s="35"/>
+      <c r="AF59" s="35"/>
+      <c r="AG59" s="35"/>
+      <c r="AH59" s="36"/>
     </row>
     <row r="60" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="15"/>
-      <c r="C60" s="33"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="33"/>
-      <c r="G60" s="33"/>
-      <c r="H60" s="33"/>
-      <c r="I60" s="33"/>
-      <c r="J60" s="33"/>
-      <c r="K60" s="33"/>
-      <c r="L60" s="33"/>
-      <c r="M60" s="33"/>
-      <c r="N60" s="33"/>
-      <c r="O60" s="33"/>
-      <c r="P60" s="33"/>
-      <c r="Q60" s="33"/>
-      <c r="R60" s="33"/>
-      <c r="S60" s="33"/>
-      <c r="T60" s="33"/>
-      <c r="U60" s="33"/>
-      <c r="V60" s="33"/>
-      <c r="W60" s="33"/>
-      <c r="X60" s="33"/>
-      <c r="Y60" s="33"/>
-      <c r="Z60" s="33"/>
-      <c r="AA60" s="33"/>
-      <c r="AB60" s="33"/>
-      <c r="AC60" s="33"/>
-      <c r="AD60" s="33"/>
-      <c r="AE60" s="33"/>
-      <c r="AF60" s="33"/>
-      <c r="AG60" s="33"/>
-      <c r="AH60" s="34"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="35"/>
+      <c r="E60" s="35"/>
+      <c r="F60" s="35"/>
+      <c r="G60" s="35"/>
+      <c r="H60" s="35"/>
+      <c r="I60" s="35"/>
+      <c r="J60" s="35"/>
+      <c r="K60" s="35"/>
+      <c r="L60" s="35"/>
+      <c r="M60" s="35"/>
+      <c r="N60" s="35"/>
+      <c r="O60" s="35"/>
+      <c r="P60" s="35"/>
+      <c r="Q60" s="35"/>
+      <c r="R60" s="35"/>
+      <c r="S60" s="35"/>
+      <c r="T60" s="35"/>
+      <c r="U60" s="35"/>
+      <c r="V60" s="35"/>
+      <c r="W60" s="35"/>
+      <c r="X60" s="35"/>
+      <c r="Y60" s="35"/>
+      <c r="Z60" s="35"/>
+      <c r="AA60" s="35"/>
+      <c r="AB60" s="35"/>
+      <c r="AC60" s="35"/>
+      <c r="AD60" s="35"/>
+      <c r="AE60" s="35"/>
+      <c r="AF60" s="35"/>
+      <c r="AG60" s="35"/>
+      <c r="AH60" s="36"/>
     </row>
     <row r="61" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="15"/>
-      <c r="C61" s="33"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="33"/>
-      <c r="F61" s="33"/>
-      <c r="G61" s="33"/>
-      <c r="H61" s="33"/>
-      <c r="I61" s="33"/>
-      <c r="J61" s="33"/>
-      <c r="K61" s="33"/>
-      <c r="L61" s="33"/>
-      <c r="M61" s="33"/>
-      <c r="N61" s="33"/>
-      <c r="O61" s="33"/>
-      <c r="P61" s="33"/>
-      <c r="Q61" s="33"/>
-      <c r="R61" s="33"/>
-      <c r="S61" s="33"/>
-      <c r="T61" s="33"/>
-      <c r="U61" s="33"/>
-      <c r="V61" s="33"/>
-      <c r="W61" s="33"/>
-      <c r="X61" s="33"/>
-      <c r="Y61" s="33"/>
-      <c r="Z61" s="33"/>
-      <c r="AA61" s="33"/>
-      <c r="AB61" s="33"/>
-      <c r="AC61" s="33"/>
-      <c r="AD61" s="33"/>
-      <c r="AE61" s="33"/>
-      <c r="AF61" s="33"/>
-      <c r="AG61" s="33"/>
-      <c r="AH61" s="34"/>
+      <c r="C61" s="35"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="35"/>
+      <c r="H61" s="35"/>
+      <c r="I61" s="35"/>
+      <c r="J61" s="35"/>
+      <c r="K61" s="35"/>
+      <c r="L61" s="35"/>
+      <c r="M61" s="35"/>
+      <c r="N61" s="35"/>
+      <c r="O61" s="35"/>
+      <c r="P61" s="35"/>
+      <c r="Q61" s="35"/>
+      <c r="R61" s="35"/>
+      <c r="S61" s="35"/>
+      <c r="T61" s="35"/>
+      <c r="U61" s="35"/>
+      <c r="V61" s="35"/>
+      <c r="W61" s="35"/>
+      <c r="X61" s="35"/>
+      <c r="Y61" s="35"/>
+      <c r="Z61" s="35"/>
+      <c r="AA61" s="35"/>
+      <c r="AB61" s="35"/>
+      <c r="AC61" s="35"/>
+      <c r="AD61" s="35"/>
+      <c r="AE61" s="35"/>
+      <c r="AF61" s="35"/>
+      <c r="AG61" s="35"/>
+      <c r="AH61" s="36"/>
     </row>
     <row r="62" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="15"/>
-      <c r="C62" s="33"/>
-      <c r="D62" s="33"/>
-      <c r="E62" s="33"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="33"/>
-      <c r="H62" s="33"/>
-      <c r="I62" s="33"/>
-      <c r="J62" s="33"/>
-      <c r="K62" s="33"/>
-      <c r="L62" s="33"/>
-      <c r="M62" s="33"/>
-      <c r="N62" s="33"/>
-      <c r="O62" s="33"/>
-      <c r="P62" s="33"/>
-      <c r="Q62" s="33"/>
-      <c r="R62" s="33"/>
-      <c r="S62" s="33"/>
-      <c r="T62" s="33"/>
-      <c r="U62" s="33"/>
-      <c r="V62" s="33"/>
-      <c r="W62" s="33"/>
-      <c r="X62" s="33"/>
-      <c r="Y62" s="33"/>
-      <c r="Z62" s="33"/>
-      <c r="AA62" s="33"/>
-      <c r="AB62" s="33"/>
-      <c r="AC62" s="33"/>
-      <c r="AD62" s="33"/>
-      <c r="AE62" s="33"/>
-      <c r="AF62" s="33"/>
-      <c r="AG62" s="33"/>
-      <c r="AH62" s="34"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="35"/>
+      <c r="H62" s="35"/>
+      <c r="I62" s="35"/>
+      <c r="J62" s="35"/>
+      <c r="K62" s="35"/>
+      <c r="L62" s="35"/>
+      <c r="M62" s="35"/>
+      <c r="N62" s="35"/>
+      <c r="O62" s="35"/>
+      <c r="P62" s="35"/>
+      <c r="Q62" s="35"/>
+      <c r="R62" s="35"/>
+      <c r="S62" s="35"/>
+      <c r="T62" s="35"/>
+      <c r="U62" s="35"/>
+      <c r="V62" s="35"/>
+      <c r="W62" s="35"/>
+      <c r="X62" s="35"/>
+      <c r="Y62" s="35"/>
+      <c r="Z62" s="35"/>
+      <c r="AA62" s="35"/>
+      <c r="AB62" s="35"/>
+      <c r="AC62" s="35"/>
+      <c r="AD62" s="35"/>
+      <c r="AE62" s="35"/>
+      <c r="AF62" s="35"/>
+      <c r="AG62" s="35"/>
+      <c r="AH62" s="36"/>
     </row>
     <row r="63" spans="2:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="15"/>
-      <c r="C63" s="33"/>
-      <c r="D63" s="33"/>
-      <c r="E63" s="33"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="33"/>
-      <c r="H63" s="33"/>
-      <c r="I63" s="33"/>
-      <c r="J63" s="33"/>
-      <c r="K63" s="33"/>
-      <c r="L63" s="33"/>
-      <c r="M63" s="33"/>
-      <c r="N63" s="33"/>
-      <c r="O63" s="33"/>
-      <c r="P63" s="33"/>
-      <c r="Q63" s="33"/>
-      <c r="R63" s="33"/>
-      <c r="S63" s="33"/>
-      <c r="T63" s="33"/>
-      <c r="U63" s="33"/>
-      <c r="V63" s="33"/>
-      <c r="W63" s="33"/>
-      <c r="X63" s="33"/>
-      <c r="Y63" s="33"/>
-      <c r="Z63" s="33"/>
-      <c r="AA63" s="33"/>
-      <c r="AB63" s="33"/>
-      <c r="AC63" s="33"/>
-      <c r="AD63" s="33"/>
-      <c r="AE63" s="33"/>
-      <c r="AF63" s="33"/>
-      <c r="AG63" s="33"/>
-      <c r="AH63" s="34"/>
+      <c r="C63" s="35"/>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="35"/>
+      <c r="H63" s="35"/>
+      <c r="I63" s="35"/>
+      <c r="J63" s="35"/>
+      <c r="K63" s="35"/>
+      <c r="L63" s="35"/>
+      <c r="M63" s="35"/>
+      <c r="N63" s="35"/>
+      <c r="O63" s="35"/>
+      <c r="P63" s="35"/>
+      <c r="Q63" s="35"/>
+      <c r="R63" s="35"/>
+      <c r="S63" s="35"/>
+      <c r="T63" s="35"/>
+      <c r="U63" s="35"/>
+      <c r="V63" s="35"/>
+      <c r="W63" s="35"/>
+      <c r="X63" s="35"/>
+      <c r="Y63" s="35"/>
+      <c r="Z63" s="35"/>
+      <c r="AA63" s="35"/>
+      <c r="AB63" s="35"/>
+      <c r="AC63" s="35"/>
+      <c r="AD63" s="35"/>
+      <c r="AE63" s="35"/>
+      <c r="AF63" s="35"/>
+      <c r="AG63" s="35"/>
+      <c r="AH63" s="36"/>
     </row>
     <row r="64" spans="2:34" ht="15" x14ac:dyDescent="0.25">
       <c r="B64" s="15"/>
@@ -2733,7 +2691,6 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2918,21 +2875,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C341BEE4C9A91F44BB4A4EF8E0A71E02" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db93f7cdcc50be3ddb7642c8d50e9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="878aac0c-df32-40a9-a231-d93e9c7b9b1a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b63aaf3684aa43c37ed0cc1f5c2cf36e" ns3:_="">
     <xsd:import namespace="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
@@ -3076,7 +3018,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9D266F6-4EBB-4FCE-8CE5-50B9641EB015}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D65B96D-4012-4621-9665-52F685045C2D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
@@ -3092,28 +3067,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8A951E8-5D72-42FD-8030-87DD7D8D4010}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9D266F6-4EBB-4FCE-8CE5-50B9641EB015}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="878aac0c-df32-40a9-a231-d93e9c7b9b1a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>